<commit_message>
graph prepared for every medicine
</commit_message>
<xml_diff>
--- a/data/merged_medicine_data.xlsx
+++ b/data/merged_medicine_data.xlsx
@@ -839,7 +839,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1238,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>